<commit_message>
added a little analysis to Excel and slightly modified code. Renamed GM folder
</commit_message>
<xml_diff>
--- a/Project Evaluation Data.xlsx
+++ b/Project Evaluation Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yashan/Documents/EECS486/finalProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benrathi/Desktop/College_Senior/Winter 2017/EECS 486/Project/code/EECS486project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" calcMode="autoNoTable" iterate="1" iterateCount="1000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>GM</t>
   </si>
@@ -50,7 +50,52 @@
     <t>% Change</t>
   </si>
   <si>
-    <t>% positivity</t>
+    <t>% Change 4/3-4/10</t>
+  </si>
+  <si>
+    <t>Accurate?</t>
+  </si>
+  <si>
+    <t>Correlation:</t>
+  </si>
+  <si>
+    <t>IPD (Auto Industry ETF)</t>
+  </si>
+  <si>
+    <t>Average of 5 stocks:</t>
+  </si>
+  <si>
+    <t>% positivity (all tweets)</t>
+  </si>
+  <si>
+    <t>% positivity ( &gt; 1000)</t>
+  </si>
+  <si>
+    <t>% positivity ( &gt; 10000)</t>
+  </si>
+  <si>
+    <t>Evaluation:</t>
+  </si>
+  <si>
+    <t>-Correlation between % change (week) and % positivity</t>
+  </si>
+  <si>
+    <t>-Accuracy (whether sign of our prediction matches weekly price movement)</t>
+  </si>
+  <si>
+    <t>Analysis:</t>
+  </si>
+  <si>
+    <t>-Follower count(s) correlations</t>
+  </si>
+  <si>
+    <t>-Industry correlation (auto ETF) with each stock</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>-"The greater the % change, the further our model is"</t>
   </si>
 </sst>
 </file>
@@ -69,16 +114,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Menlo"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,12 +149,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,56 +433,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="18.33203125" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="4">
         <v>42828</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="4">
         <v>42829</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="4">
         <v>42830</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1" s="4">
         <v>42831</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="4">
         <v>42832</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1" s="4">
         <v>42835</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -475,11 +553,38 @@
       <c r="L2">
         <v>33.97</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="1">
+        <f>(L2-B2)/B2</f>
+        <v>-5.8530875036582625E-3</v>
+      </c>
+      <c r="N2" s="1">
         <v>-1.6299999999999999E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O2" t="str">
+        <f>IF(OR(AND(N2&gt;0,$M2&gt;0),AND(N2&lt;0,$M2&lt;0)),"YES","NO")</f>
+        <v>YES</v>
+      </c>
+      <c r="P2" s="1">
+        <f>ABS(N2-M2)</f>
+        <v>1.0446912496341736E-2</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>-3.31E-3</v>
+      </c>
+      <c r="R2" t="str">
+        <f>IF(OR(AND(Q2&gt;0,$M2&gt;0),AND(Q2&lt;0,$M2&lt;0)),"YES","NO")</f>
+        <v>YES</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1.46E-2</v>
+      </c>
+      <c r="T2" t="str">
+        <f>IF(OR(AND(S2&gt;0,$M2&gt;0),AND(S2&lt;0,$M2&lt;0)),"YES","NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="U2" s="1"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -487,45 +592,72 @@
         <v>11.44</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C6" si="0">(D3-B3)/B3*100</f>
+        <f t="shared" ref="C3:C7" si="0">(D3-B3)/B3*100</f>
         <v>-0.61188811188811443</v>
       </c>
       <c r="D3">
         <v>11.37</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E6" si="1">(F3-D3)/D3*100</f>
+        <f t="shared" ref="E3:E7" si="1">(F3-D3)/D3*100</f>
         <v>-0.96745822339489396</v>
       </c>
       <c r="F3">
         <v>11.26</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G6" si="2">(H3-F3)/F3*100</f>
+        <f t="shared" ref="G3:G7" si="2">(H3-F3)/F3*100</f>
         <v>8.8809946714030072E-2</v>
       </c>
       <c r="H3">
         <v>11.27</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I6" si="3">(J3-H3)/H3*100</f>
+        <f t="shared" ref="I3:I7" si="3">(J3-H3)/H3*100</f>
         <v>-0.35492457852705545</v>
       </c>
       <c r="J3">
         <v>11.23</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K6" si="4">(L3-J3)/J3*100</f>
+        <f t="shared" ref="K3:K7" si="4">(L3-J3)/J3*100</f>
         <v>0.17809439002671035</v>
       </c>
       <c r="L3">
         <v>11.25</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="1">
+        <f>(L3-B3)/B3</f>
+        <v>-1.6608391608391566E-2</v>
+      </c>
+      <c r="N3" s="1">
         <v>7.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O3" t="str">
+        <f t="shared" ref="O3" si="5">IF(OR(AND(N3&gt;0,$M3&gt;0),AND(N3&lt;0,$M3&lt;0)),"YES","NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" ref="P3:P6" si="6">ABS(N3-M3)</f>
+        <v>2.4108391608391566E-2</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>6.3499999999999997E-3</v>
+      </c>
+      <c r="R3" t="str">
+        <f t="shared" ref="R3:T6" si="7">IF(OR(AND(Q3&gt;0,$M3&gt;0),AND(Q3&lt;0,$M3&lt;0)),"YES","NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="S3" s="1">
+        <v>-1.6629999999999999E-2</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" si="7"/>
+        <v>YES</v>
+      </c>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -567,11 +699,38 @@
       <c r="L4">
         <v>29.6</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:M7" si="8">(L4-B4)/B4</f>
+        <v>-1.2345679012345593E-2</v>
+      </c>
+      <c r="N4" s="1">
         <v>8.8000000000000005E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O4" t="str">
+        <f t="shared" ref="O4" si="9">IF(OR(AND(N4&gt;0,$M4&gt;0),AND(N4&lt;0,$M4&lt;0)),"YES","NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" si="6"/>
+        <v>2.1145679012345594E-2</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>2.3560000000000001E-2</v>
+      </c>
+      <c r="R4" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+      <c r="S4" s="1">
+        <v>3.49E-2</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -613,11 +772,38 @@
       <c r="L5">
         <v>105.98</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="1">
+        <f t="shared" si="8"/>
+        <v>-2.3405823811278953E-2</v>
+      </c>
+      <c r="N5" s="1">
         <v>7.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O5" t="str">
+        <f t="shared" ref="O5" si="10">IF(OR(AND(N5&gt;0,$M5&gt;0),AND(N5&lt;0,$M5&lt;0)),"YES","NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="6"/>
+        <v>3.0605823811278951E-2</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>5.1200000000000004E-3</v>
+      </c>
+      <c r="R5" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+      <c r="S5" s="1">
+        <v>4.4749999999999998E-2</v>
+      </c>
+      <c r="T5" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -659,8 +845,158 @@
       <c r="L6">
         <v>312.39</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="1">
+        <f t="shared" si="8"/>
+        <v>4.6462548572959957E-2</v>
+      </c>
+      <c r="N6" s="1">
         <v>6.5399999999999998E-3</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" ref="O6" si="11">IF(OR(AND(N6&gt;0,$M6&gt;0),AND(N6&lt;0,$M6&lt;0)),"YES","NO")</f>
+        <v>YES</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="6"/>
+        <v>3.9922548572959959E-2</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1.231E-2</v>
+      </c>
+      <c r="R6" t="str">
+        <f t="shared" si="7"/>
+        <v>YES</v>
+      </c>
+      <c r="S6" s="1">
+        <v>2.3650000000000001E-2</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="7"/>
+        <v>YES</v>
+      </c>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="1">
+        <f>AVERAGE(M2:M6)</f>
+        <v>-2.3500866725428837E-3</v>
+      </c>
+      <c r="N7" s="1">
+        <f>AVERAGE(N2:N6)</f>
+        <v>2.7480000000000004E-3</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1">
+        <f>AVERAGE(Q2:Q6)</f>
+        <v>8.8060000000000013E-3</v>
+      </c>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1">
+        <f>AVERAGE(S2:S6)</f>
+        <v>2.0254000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>37.96</v>
+      </c>
+      <c r="C9">
+        <f>(D9-B9)/B9*100</f>
+        <v>-0.23709167544784882</v>
+      </c>
+      <c r="D9">
+        <v>37.869999999999997</v>
+      </c>
+      <c r="E9">
+        <f>(F9-D9)/D9*100</f>
+        <v>-0.44890414576180249</v>
+      </c>
+      <c r="F9">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="G9">
+        <f>(H9-F9)/F9*100</f>
+        <v>-0.13262599469497149</v>
+      </c>
+      <c r="H9">
+        <v>37.65</v>
+      </c>
+      <c r="I9">
+        <f>(J9-H9)/H9*100</f>
+        <v>-0.15936254980078399</v>
+      </c>
+      <c r="J9">
+        <v>37.590000000000003</v>
+      </c>
+      <c r="K9">
+        <f>(L9-J9)/J9*100</f>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>37.590000000000003</v>
+      </c>
+      <c r="M9" s="1">
+        <f>(L9-B9)/B9</f>
+        <v>-9.7471022128555705E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="M11" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <f>CORREL(M2:M6,N2:N6)</f>
+        <v>2.4919845879028381E-2</v>
+      </c>
+      <c r="Q11">
+        <f>CORREL(M2:M6,Q2:Q6)</f>
+        <v>0.1600845194782988</v>
+      </c>
+      <c r="S11">
+        <f>CORREL(M2:M6,S2:S6)</f>
+        <v>1.8674613466391494E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>